<commit_message>
create tutorial for training and evaluating bpr
</commit_message>
<xml_diff>
--- a/docs/notebooks/data/ct-lymph-nodes-annotated-landmarks.xlsx
+++ b/docs/notebooks/data/ct-lymph-nodes-annotated-landmarks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="landmarks-train" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t xml:space="preserve">filename</t>
   </si>
@@ -56,118 +56,91 @@
     <t xml:space="preserve">Th2</t>
   </si>
   <si>
+    <t xml:space="preserve">ABD_LYMPH_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABD_LYMPH_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABD_LYMPH_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED_LYMPH_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABD_LYMPH_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABD_LYMPH_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABD_LYMPH_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABD_LYMPH_005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED_LYMPH_001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED_LYMPH_002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED_LYMPH_003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED_LYMPH_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pelvis_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kidney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lung_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liver_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lung_end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Th1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7</t>
+  </si>
+  <si>
     <t xml:space="preserve">C6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED_LYMPH_006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABD_LYMPH_005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED_LYMPH_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED_LYMPH_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED_LYMPH_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MED_LYMPH_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pelvis_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kidney</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lung_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liver_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lung_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">teeth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eyes_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">head_end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Th1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
   </si>
   <si>
     <t xml:space="preserve">val</t>
@@ -346,16 +319,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="2" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -389,13 +363,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>14</v>
@@ -424,7 +395,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>69</v>
@@ -456,7 +427,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>38</v>
@@ -488,7 +459,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>10</v>
@@ -516,9 +487,6 @@
       </c>
       <c r="J5" s="0" t="n">
         <v>615</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -537,15 +505,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,13 +548,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>27</v>
@@ -614,13 +580,10 @@
       <c r="J2" s="0" t="n">
         <v>611</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>652</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
@@ -646,7 +609,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -675,13 +638,10 @@
       <c r="J4" s="0" t="n">
         <v>685</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <v>731</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>41</v>
@@ -713,7 +673,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -745,7 +705,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>27</v>
@@ -774,13 +734,10 @@
       <c r="J7" s="0" t="n">
         <v>611</v>
       </c>
-      <c r="K7" s="0" t="n">
-        <v>654</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>93</v>
@@ -809,7 +766,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>27</v>
@@ -834,9 +791,6 @@
       </c>
       <c r="J9" s="0" t="n">
         <v>645</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -855,15 +809,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -897,13 +852,10 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>27</v>
@@ -932,13 +884,10 @@
       <c r="J2" s="0" t="n">
         <v>611</v>
       </c>
-      <c r="K2" s="0" t="n">
-        <v>652</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
@@ -964,7 +913,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -993,13 +942,10 @@
       <c r="J4" s="0" t="n">
         <v>685</v>
       </c>
-      <c r="K4" s="0" t="n">
-        <v>731</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>41</v>
@@ -1031,7 +977,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1063,7 +1009,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>27</v>
@@ -1092,13 +1038,10 @@
       <c r="J7" s="0" t="n">
         <v>611</v>
       </c>
-      <c r="K7" s="0" t="n">
-        <v>654</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>93</v>
@@ -1127,7 +1070,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>27</v>
@@ -1152,9 +1095,6 @@
       </c>
       <c r="J9" s="0" t="n">
         <v>645</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -1173,13 +1113,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM13"/>
+  <dimension ref="A1:AD13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA7" activeCellId="0" sqref="AA7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.02"/>
   </cols>
@@ -1195,117 +1135,90 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>27</v>
@@ -1328,76 +1241,76 @@
       <c r="H2" s="0" t="n">
         <v>636</v>
       </c>
+      <c r="I2" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>244</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>279</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>313</v>
+      </c>
       <c r="M2" s="0" t="n">
-        <v>210</v>
+        <v>345</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>244</v>
+        <v>377</v>
       </c>
       <c r="O2" s="0" t="n">
-        <v>279</v>
+        <v>407</v>
       </c>
       <c r="P2" s="0" t="n">
-        <v>313</v>
+        <v>436</v>
       </c>
       <c r="Q2" s="0" t="n">
-        <v>345</v>
+        <v>462</v>
       </c>
       <c r="R2" s="0" t="n">
-        <v>377</v>
+        <v>488</v>
       </c>
       <c r="S2" s="0" t="n">
-        <v>407</v>
+        <v>509</v>
       </c>
       <c r="T2" s="0" t="n">
-        <v>436</v>
+        <v>532</v>
       </c>
       <c r="U2" s="0" t="n">
-        <v>462</v>
+        <v>554</v>
       </c>
       <c r="V2" s="0" t="n">
-        <v>488</v>
+        <v>575</v>
       </c>
       <c r="W2" s="0" t="n">
-        <v>509</v>
+        <v>594</v>
       </c>
       <c r="X2" s="0" t="n">
-        <v>532</v>
+        <v>611</v>
       </c>
       <c r="Y2" s="0" t="n">
-        <v>554</v>
+        <v>627</v>
       </c>
       <c r="Z2" s="0" t="n">
-        <v>575</v>
+        <v>641</v>
       </c>
       <c r="AA2" s="0" t="n">
-        <v>594</v>
+        <v>652</v>
       </c>
       <c r="AB2" s="0" t="n">
-        <v>611</v>
+        <v>1</v>
       </c>
       <c r="AC2" s="0" t="n">
-        <v>627</v>
+        <v>0</v>
       </c>
       <c r="AD2" s="0" t="n">
-        <v>641</v>
-      </c>
-      <c r="AE2" s="0" t="n">
-        <v>652</v>
-      </c>
-      <c r="AK2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
@@ -1417,49 +1330,49 @@
       <c r="G3" s="0" t="n">
         <v>466</v>
       </c>
+      <c r="I3" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>229</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>297</v>
+      </c>
       <c r="M3" s="0" t="n">
-        <v>198</v>
+        <v>331</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>229</v>
+        <v>364</v>
       </c>
       <c r="O3" s="0" t="n">
-        <v>263</v>
+        <v>395</v>
       </c>
       <c r="P3" s="0" t="n">
-        <v>297</v>
+        <v>424</v>
       </c>
       <c r="Q3" s="0" t="n">
-        <v>331</v>
+        <v>449</v>
       </c>
       <c r="R3" s="0" t="n">
-        <v>364</v>
-      </c>
-      <c r="S3" s="0" t="n">
-        <v>395</v>
-      </c>
-      <c r="T3" s="0" t="n">
-        <v>424</v>
-      </c>
-      <c r="U3" s="0" t="n">
-        <v>449</v>
-      </c>
-      <c r="V3" s="0" t="n">
         <v>474</v>
       </c>
-      <c r="AK3" s="0" t="n">
+      <c r="AB3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="AL3" s="0" t="n">
+      <c r="AC3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AM3" s="0" t="n">
+      <c r="AD3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -1482,76 +1395,76 @@
       <c r="H4" s="0" t="n">
         <v>705</v>
       </c>
+      <c r="I4" s="0" t="n">
+        <v>235</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>267</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>303</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>339</v>
+      </c>
       <c r="M4" s="0" t="n">
-        <v>235</v>
+        <v>378</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>267</v>
+        <v>415</v>
       </c>
       <c r="O4" s="0" t="n">
-        <v>303</v>
+        <v>448</v>
       </c>
       <c r="P4" s="0" t="n">
-        <v>339</v>
+        <v>478</v>
       </c>
       <c r="Q4" s="0" t="n">
-        <v>378</v>
+        <v>506</v>
       </c>
       <c r="R4" s="0" t="n">
-        <v>415</v>
+        <v>533</v>
       </c>
       <c r="S4" s="0" t="n">
-        <v>448</v>
+        <v>560</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>478</v>
+        <v>586</v>
       </c>
       <c r="U4" s="0" t="n">
-        <v>506</v>
+        <v>612</v>
       </c>
       <c r="V4" s="0" t="n">
-        <v>533</v>
+        <v>637</v>
       </c>
       <c r="W4" s="0" t="n">
-        <v>560</v>
+        <v>662</v>
       </c>
       <c r="X4" s="0" t="n">
-        <v>586</v>
+        <v>685</v>
       </c>
       <c r="Y4" s="0" t="n">
-        <v>612</v>
+        <v>706</v>
       </c>
       <c r="Z4" s="0" t="n">
-        <v>637</v>
+        <v>724</v>
       </c>
       <c r="AA4" s="0" t="n">
-        <v>662</v>
+        <v>731</v>
       </c>
       <c r="AB4" s="0" t="n">
-        <v>685</v>
+        <v>1</v>
       </c>
       <c r="AC4" s="0" t="n">
-        <v>706</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="0" t="n">
-        <v>724</v>
-      </c>
-      <c r="AE4" s="0" t="n">
-        <v>731</v>
-      </c>
-      <c r="AK4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>41</v>
@@ -1574,70 +1487,70 @@
       <c r="H5" s="0" t="n">
         <v>638</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <v>234</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>266</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>301</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>336</v>
+      </c>
       <c r="M5" s="0" t="n">
-        <v>234</v>
+        <v>370</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>266</v>
+        <v>403</v>
       </c>
       <c r="O5" s="0" t="n">
-        <v>301</v>
+        <v>432</v>
       </c>
       <c r="P5" s="0" t="n">
-        <v>336</v>
+        <v>459</v>
       </c>
       <c r="Q5" s="0" t="n">
-        <v>370</v>
+        <v>483</v>
       </c>
       <c r="R5" s="0" t="n">
-        <v>403</v>
+        <v>505</v>
       </c>
       <c r="S5" s="0" t="n">
-        <v>432</v>
+        <v>527</v>
       </c>
       <c r="T5" s="0" t="n">
-        <v>459</v>
+        <v>550</v>
       </c>
       <c r="U5" s="0" t="n">
-        <v>483</v>
+        <v>571</v>
       </c>
       <c r="V5" s="0" t="n">
-        <v>505</v>
+        <v>591</v>
       </c>
       <c r="W5" s="0" t="n">
-        <v>527</v>
+        <v>609</v>
       </c>
       <c r="X5" s="0" t="n">
-        <v>550</v>
+        <v>628</v>
       </c>
       <c r="Y5" s="0" t="n">
-        <v>571</v>
-      </c>
-      <c r="Z5" s="0" t="n">
-        <v>591</v>
-      </c>
-      <c r="AA5" s="0" t="n">
-        <v>609</v>
+        <v>642</v>
       </c>
       <c r="AB5" s="0" t="n">
-        <v>628</v>
+        <v>1</v>
       </c>
       <c r="AC5" s="0" t="n">
-        <v>642</v>
-      </c>
-      <c r="AK5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL5" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="AM5" s="0" t="n">
+      <c r="AD5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>14</v>
@@ -1660,70 +1573,70 @@
       <c r="H6" s="0" t="n">
         <v>613</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>241</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>273</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>306</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>339</v>
+      </c>
       <c r="N6" s="0" t="n">
-        <v>241</v>
+        <v>370</v>
       </c>
       <c r="O6" s="0" t="n">
-        <v>273</v>
+        <v>400</v>
       </c>
       <c r="P6" s="0" t="n">
-        <v>306</v>
+        <v>427</v>
       </c>
       <c r="Q6" s="0" t="n">
-        <v>339</v>
+        <v>451</v>
       </c>
       <c r="R6" s="0" t="n">
-        <v>370</v>
+        <v>475</v>
       </c>
       <c r="S6" s="0" t="n">
-        <v>400</v>
+        <v>498</v>
       </c>
       <c r="T6" s="0" t="n">
-        <v>427</v>
+        <v>522</v>
       </c>
       <c r="U6" s="0" t="n">
-        <v>451</v>
+        <v>543</v>
       </c>
       <c r="V6" s="0" t="n">
-        <v>475</v>
+        <v>564</v>
       </c>
       <c r="W6" s="0" t="n">
-        <v>498</v>
+        <v>583</v>
       </c>
       <c r="X6" s="0" t="n">
-        <v>522</v>
+        <v>602</v>
       </c>
       <c r="Y6" s="0" t="n">
-        <v>543</v>
+        <v>619</v>
       </c>
       <c r="Z6" s="0" t="n">
-        <v>564</v>
-      </c>
-      <c r="AA6" s="0" t="n">
-        <v>583</v>
+        <v>632</v>
       </c>
       <c r="AB6" s="0" t="n">
-        <v>602</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="0" t="n">
-        <v>619</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="0" t="n">
-        <v>632</v>
-      </c>
-      <c r="AK6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>69</v>
@@ -1746,73 +1659,73 @@
       <c r="H7" s="0" t="n">
         <v>720</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <v>282</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>311</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>378</v>
+      </c>
       <c r="M7" s="0" t="n">
-        <v>282</v>
+        <v>412</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>311</v>
+        <v>446</v>
       </c>
       <c r="O7" s="0" t="n">
-        <v>344</v>
+        <v>479</v>
       </c>
       <c r="P7" s="0" t="n">
-        <v>378</v>
+        <v>509</v>
       </c>
       <c r="Q7" s="0" t="n">
-        <v>412</v>
+        <v>537</v>
       </c>
       <c r="R7" s="0" t="n">
-        <v>446</v>
+        <v>559</v>
       </c>
       <c r="S7" s="0" t="n">
-        <v>479</v>
+        <v>586</v>
       </c>
       <c r="T7" s="0" t="n">
-        <v>509</v>
+        <v>613</v>
       </c>
       <c r="U7" s="0" t="n">
-        <v>537</v>
+        <v>637</v>
       </c>
       <c r="V7" s="0" t="n">
-        <v>559</v>
+        <v>661</v>
       </c>
       <c r="W7" s="0" t="n">
-        <v>586</v>
+        <v>683</v>
       </c>
       <c r="X7" s="0" t="n">
-        <v>613</v>
+        <v>703</v>
       </c>
       <c r="Y7" s="0" t="n">
-        <v>637</v>
+        <v>722</v>
       </c>
       <c r="Z7" s="0" t="n">
-        <v>661</v>
-      </c>
-      <c r="AA7" s="0" t="n">
-        <v>683</v>
+        <v>737</v>
       </c>
       <c r="AB7" s="0" t="n">
-        <v>703</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="0" t="n">
-        <v>722</v>
+        <v>1</v>
       </c>
       <c r="AD7" s="0" t="n">
-        <v>737</v>
-      </c>
-      <c r="AK7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>38</v>
@@ -1835,73 +1748,73 @@
       <c r="H8" s="0" t="n">
         <v>621</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <v>216</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>245</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>276</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>306</v>
+      </c>
       <c r="M8" s="0" t="n">
-        <v>216</v>
+        <v>339</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>245</v>
+        <v>371</v>
       </c>
       <c r="O8" s="0" t="n">
-        <v>276</v>
+        <v>400</v>
       </c>
       <c r="P8" s="0" t="n">
-        <v>306</v>
+        <v>426</v>
       </c>
       <c r="Q8" s="0" t="n">
-        <v>339</v>
+        <v>450</v>
       </c>
       <c r="R8" s="0" t="n">
-        <v>371</v>
+        <v>472</v>
       </c>
       <c r="S8" s="0" t="n">
-        <v>400</v>
+        <v>494</v>
       </c>
       <c r="T8" s="0" t="n">
-        <v>426</v>
+        <v>516</v>
       </c>
       <c r="U8" s="0" t="n">
-        <v>450</v>
+        <v>538</v>
       </c>
       <c r="V8" s="0" t="n">
-        <v>472</v>
+        <v>559</v>
       </c>
       <c r="W8" s="0" t="n">
-        <v>494</v>
+        <v>579</v>
       </c>
       <c r="X8" s="0" t="n">
-        <v>516</v>
+        <v>598</v>
       </c>
       <c r="Y8" s="0" t="n">
-        <v>538</v>
+        <v>614</v>
       </c>
       <c r="Z8" s="0" t="n">
-        <v>559</v>
-      </c>
-      <c r="AA8" s="0" t="n">
-        <v>579</v>
+        <v>629</v>
       </c>
       <c r="AB8" s="0" t="n">
-        <v>598</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="0" t="n">
-        <v>614</v>
+        <v>1</v>
       </c>
       <c r="AD8" s="0" t="n">
-        <v>629</v>
-      </c>
-      <c r="AK8" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM8" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -1924,70 +1837,70 @@
       <c r="H9" s="0" t="n">
         <v>629</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>230</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>265</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>301</v>
+      </c>
       <c r="M9" s="0" t="n">
-        <v>196</v>
+        <v>335</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>230</v>
+        <v>369</v>
       </c>
       <c r="O9" s="0" t="n">
-        <v>265</v>
+        <v>401</v>
       </c>
       <c r="P9" s="0" t="n">
-        <v>301</v>
+        <v>429</v>
       </c>
       <c r="Q9" s="0" t="n">
-        <v>335</v>
+        <v>455</v>
       </c>
       <c r="R9" s="0" t="n">
-        <v>369</v>
+        <v>482</v>
       </c>
       <c r="S9" s="0" t="n">
-        <v>401</v>
+        <v>508</v>
       </c>
       <c r="T9" s="0" t="n">
-        <v>429</v>
+        <v>533</v>
       </c>
       <c r="U9" s="0" t="n">
-        <v>455</v>
+        <v>557</v>
       </c>
       <c r="V9" s="0" t="n">
-        <v>482</v>
+        <v>579</v>
       </c>
       <c r="W9" s="0" t="n">
-        <v>508</v>
+        <v>601</v>
       </c>
       <c r="X9" s="0" t="n">
-        <v>533</v>
+        <v>621</v>
       </c>
       <c r="Y9" s="0" t="n">
-        <v>557</v>
+        <v>638</v>
       </c>
       <c r="Z9" s="0" t="n">
-        <v>579</v>
-      </c>
-      <c r="AA9" s="0" t="n">
-        <v>601</v>
+        <v>654</v>
       </c>
       <c r="AB9" s="0" t="n">
-        <v>621</v>
-      </c>
-      <c r="AC9" s="0" t="n">
-        <v>638</v>
+        <v>1</v>
       </c>
       <c r="AD9" s="0" t="n">
-        <v>654</v>
-      </c>
-      <c r="AK9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>27</v>
@@ -2010,73 +1923,73 @@
       <c r="H10" s="0" t="n">
         <v>626</v>
       </c>
+      <c r="I10" s="0" t="n">
+        <v>210</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>243</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>279</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>313</v>
+      </c>
       <c r="M10" s="0" t="n">
-        <v>210</v>
+        <v>346</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>243</v>
+        <v>378</v>
       </c>
       <c r="O10" s="0" t="n">
-        <v>279</v>
+        <v>408</v>
       </c>
       <c r="P10" s="0" t="n">
-        <v>313</v>
+        <v>436</v>
       </c>
       <c r="Q10" s="0" t="n">
-        <v>346</v>
+        <v>461</v>
       </c>
       <c r="R10" s="0" t="n">
-        <v>378</v>
+        <v>486</v>
       </c>
       <c r="S10" s="0" t="n">
-        <v>408</v>
+        <v>509</v>
       </c>
       <c r="T10" s="0" t="n">
-        <v>436</v>
+        <v>532</v>
       </c>
       <c r="U10" s="0" t="n">
-        <v>461</v>
+        <v>554</v>
       </c>
       <c r="V10" s="0" t="n">
-        <v>486</v>
+        <v>575</v>
       </c>
       <c r="W10" s="0" t="n">
-        <v>509</v>
+        <v>594</v>
       </c>
       <c r="X10" s="0" t="n">
-        <v>532</v>
+        <v>611</v>
       </c>
       <c r="Y10" s="0" t="n">
-        <v>554</v>
+        <v>627</v>
       </c>
       <c r="Z10" s="0" t="n">
-        <v>575</v>
+        <v>642</v>
       </c>
       <c r="AA10" s="0" t="n">
-        <v>594</v>
+        <v>654</v>
       </c>
       <c r="AB10" s="0" t="n">
-        <v>611</v>
-      </c>
-      <c r="AC10" s="0" t="n">
-        <v>627</v>
+        <v>1</v>
       </c>
       <c r="AD10" s="0" t="n">
-        <v>642</v>
-      </c>
-      <c r="AE10" s="0" t="n">
-        <v>654</v>
-      </c>
-      <c r="AK10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>93</v>
@@ -2099,67 +2012,67 @@
       <c r="H11" s="0" t="n">
         <v>731</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <v>308</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>375</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>410</v>
+      </c>
       <c r="M11" s="0" t="n">
-        <v>308</v>
+        <v>445</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>342</v>
-      </c>
-      <c r="O11" s="0" t="n">
-        <v>375</v>
+        <v>479</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>410</v>
+        <v>538</v>
       </c>
       <c r="Q11" s="0" t="n">
-        <v>445</v>
+        <v>564</v>
       </c>
       <c r="R11" s="0" t="n">
-        <v>479</v>
+        <v>588</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>613</v>
       </c>
       <c r="T11" s="0" t="n">
-        <v>538</v>
+        <v>636</v>
       </c>
       <c r="U11" s="0" t="n">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="V11" s="0" t="n">
-        <v>588</v>
+        <v>679</v>
       </c>
       <c r="W11" s="0" t="n">
-        <v>613</v>
+        <v>698</v>
       </c>
       <c r="X11" s="0" t="n">
-        <v>636</v>
+        <v>718</v>
       </c>
       <c r="Y11" s="0" t="n">
-        <v>658</v>
+        <v>737</v>
       </c>
       <c r="Z11" s="0" t="n">
-        <v>679</v>
-      </c>
-      <c r="AA11" s="0" t="n">
-        <v>698</v>
+        <v>750</v>
       </c>
       <c r="AB11" s="0" t="n">
-        <v>718</v>
-      </c>
-      <c r="AC11" s="0" t="n">
-        <v>737</v>
+        <v>1</v>
       </c>
       <c r="AD11" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="AK11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>27</v>
@@ -2182,70 +2095,70 @@
       <c r="H12" s="0" t="n">
         <v>658</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <v>231</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>263</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>297</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>331</v>
+      </c>
       <c r="M12" s="0" t="n">
-        <v>231</v>
+        <v>365</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>263</v>
-      </c>
-      <c r="O12" s="0" t="n">
-        <v>297</v>
+        <v>397</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>331</v>
+        <v>456</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>365</v>
+        <v>483</v>
       </c>
       <c r="R12" s="0" t="n">
-        <v>397</v>
+        <v>508</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>532</v>
       </c>
       <c r="T12" s="0" t="n">
-        <v>456</v>
+        <v>555</v>
       </c>
       <c r="U12" s="0" t="n">
-        <v>483</v>
+        <v>578</v>
       </c>
       <c r="V12" s="0" t="n">
-        <v>508</v>
+        <v>601</v>
       </c>
       <c r="W12" s="0" t="n">
-        <v>532</v>
+        <v>623</v>
       </c>
       <c r="X12" s="0" t="n">
-        <v>555</v>
+        <v>645</v>
       </c>
       <c r="Y12" s="0" t="n">
-        <v>578</v>
+        <v>664</v>
       </c>
       <c r="Z12" s="0" t="n">
-        <v>601</v>
+        <v>679</v>
       </c>
       <c r="AA12" s="0" t="n">
-        <v>623</v>
+        <v>695</v>
       </c>
       <c r="AB12" s="0" t="n">
-        <v>645</v>
-      </c>
-      <c r="AC12" s="0" t="n">
-        <v>664</v>
+        <v>1</v>
       </c>
       <c r="AD12" s="0" t="n">
-        <v>679</v>
-      </c>
-      <c r="AE12" s="0" t="n">
-        <v>695</v>
-      </c>
-      <c r="AK12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>10</v>
@@ -2268,64 +2181,64 @@
       <c r="H13" s="0" t="n">
         <v>632</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <v>205</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>238</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>272</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>306</v>
+      </c>
       <c r="M13" s="0" t="n">
-        <v>205</v>
+        <v>340</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>238</v>
+        <v>372</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>272</v>
+        <v>402</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>306</v>
+        <v>430</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>340</v>
+        <v>456</v>
       </c>
       <c r="R13" s="0" t="n">
-        <v>372</v>
+        <v>481</v>
       </c>
       <c r="S13" s="0" t="n">
-        <v>402</v>
+        <v>505</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>430</v>
+        <v>529</v>
       </c>
       <c r="U13" s="0" t="n">
-        <v>456</v>
+        <v>552</v>
       </c>
       <c r="V13" s="0" t="n">
-        <v>481</v>
+        <v>574</v>
       </c>
       <c r="W13" s="0" t="n">
-        <v>505</v>
+        <v>595</v>
       </c>
       <c r="X13" s="0" t="n">
-        <v>529</v>
+        <v>615</v>
       </c>
       <c r="Y13" s="0" t="n">
-        <v>552</v>
+        <v>634</v>
       </c>
       <c r="Z13" s="0" t="n">
-        <v>574</v>
+        <v>650</v>
       </c>
       <c r="AA13" s="0" t="n">
-        <v>595</v>
-      </c>
-      <c r="AB13" s="0" t="n">
-        <v>615</v>
+        <v>666</v>
       </c>
       <c r="AC13" s="0" t="n">
-        <v>634</v>
-      </c>
-      <c r="AD13" s="0" t="n">
-        <v>650</v>
-      </c>
-      <c r="AE13" s="0" t="n">
-        <v>666</v>
-      </c>
-      <c r="AL13" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2360,49 +2273,49 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>